<commit_message>
2015.06.05 Add Window Icon
</commit_message>
<xml_diff>
--- a/docs/記憶構造.xlsx
+++ b/docs/記憶構造.xlsx
@@ -83,143 +83,9 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>namespaceがApp1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Systemを使っている</t>
     <rPh sb="7" eb="8">
       <t>ツカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>クラス名が　Program</t>
-    <rPh sb="3" eb="4">
-      <t>メイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>関数情報：記憶クラス=static、戻り値=void、名称=Main、引数=args[]、引数の型=Object</t>
-    <rPh sb="0" eb="2">
-      <t>カンスウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>キオク</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>モド</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>チ</t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t>メイショウ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>ヒキスウ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ヒキスウ</t>
-    </rPh>
-    <rPh sb="48" eb="49">
-      <t>カタ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>プログラムステップ　ステップタイプ=代入、非代入変数=i、非代入変数の型=var、代入値=arg[0]</t>
-    <rPh sb="18" eb="20">
-      <t>ダイニュウ</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>ヒ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ダイニュウ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ヘンスウ</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>ヒ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>ダイニュウ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>ヘンスウ</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>カタ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>ダイニュウ</t>
-    </rPh>
-    <rPh sb="43" eb="44">
-      <t>チ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>プログラムステップ　ステップタイプ=関数呼び出し、結果代入変数=v、結果代入変数の型=int、呼び出しメソッド名=func1、呼び出し引数=i、引数の型=var</t>
-    <rPh sb="18" eb="20">
-      <t>カンスウ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="22" eb="23">
-      <t>ダ</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>ケッカ</t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t>ダイニュウ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>ヘンスウ</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>ケッカ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>ダイニュウ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>ヘンスウ</t>
-    </rPh>
-    <rPh sb="41" eb="42">
-      <t>カタ</t>
-    </rPh>
-    <rPh sb="47" eb="48">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="49" eb="50">
-      <t>ダ</t>
-    </rPh>
-    <rPh sb="55" eb="56">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="63" eb="64">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="65" eb="66">
-      <t>ダ</t>
-    </rPh>
-    <rPh sb="67" eb="69">
-      <t>ヒキスウ</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>ヒキスウ</t>
-    </rPh>
-    <rPh sb="75" eb="76">
-      <t>カタ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -234,71 +100,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>関数情報：記憶クラス=auto、メンバアクセス修飾子=protected、戻り値=int、名称=func1、仮引数=aInt、仮引数の型=int</t>
-    <rPh sb="0" eb="2">
-      <t>カンスウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>キオク</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>シュウショク</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>シ</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>モド</t>
-    </rPh>
-    <rPh sb="39" eb="40">
-      <t>チ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>メイショウ</t>
-    </rPh>
-    <rPh sb="54" eb="55">
-      <t>カリ</t>
-    </rPh>
-    <rPh sb="55" eb="57">
-      <t>ヒキスウ</t>
-    </rPh>
-    <rPh sb="63" eb="64">
-      <t>カリ</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>ヒキスウ</t>
-    </rPh>
-    <rPh sb="67" eb="68">
-      <t>カタ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>プログラムステップ　ステップタイプ=復帰、復帰値=aInt、復帰値の型=int</t>
-    <rPh sb="18" eb="20">
-      <t>フッキ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>フッキ</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>チ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>フッキ</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>チ</t>
-    </rPh>
-    <rPh sb="34" eb="35">
-      <t>カタ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>こんな感じで記憶したい</t>
     <rPh sb="3" eb="4">
       <t>カン</t>
@@ -312,6 +113,241 @@
     <t>例題ソース</t>
     <rPh sb="0" eb="2">
       <t>レイダイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">関数情報：
+記憶クラス=static
+戻り値=void
+名称=Main
+引数=args[]
+引数の型=Object
+</t>
+    <rPh sb="0" eb="2">
+      <t>カンスウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>キオク</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>チ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>メイショウ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="49" eb="50">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">クラス：
+名称=Program
+</t>
+    <rPh sb="5" eb="7">
+      <t>メイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">namespace：
+名称=App1
+</t>
+    <rPh sb="11" eb="13">
+      <t>メイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">プログラムステップ：
+ステップタイプ=代入
+非代入変数=I
+非代入変数の型=var
+代入値=arg[0]
+</t>
+    <rPh sb="19" eb="21">
+      <t>ダイニュウ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ヒ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ダイニュウ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>ヒ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>ダイニュウ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ダイニュウ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">プログラムステップ：
+ステップタイプ=関数呼び出し
+結果代入変数=v
+結果代入変数の型=int
+呼び出しメソッド名=func1
+呼び出し引数=I
+引数の型=var
+</t>
+    <rPh sb="19" eb="21">
+      <t>カンスウ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ケッカ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ダイニュウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ケッカ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ダイニュウ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="76" eb="77">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">関数情報：
+記憶クラス=auto
+メンバアクセス修飾子=protected
+戻り値=int
+名称=func1
+仮引数=aInt
+仮引数の型=int
+</t>
+    <rPh sb="0" eb="2">
+      <t>カンスウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>キオク</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>シュウショク</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>チ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>メイショウ</t>
+    </rPh>
+    <rPh sb="55" eb="56">
+      <t>カリ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>カリ</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="68" eb="69">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">プログラムステップ：
+ステップタイプ=復帰
+復帰値=aInt
+復帰値の型=int
+</t>
+    <rPh sb="19" eb="21">
+      <t>フッキ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>フッキ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>チ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>フッキ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>チ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>カタ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -359,9 +395,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2398,141 +2440,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:F24"/>
+  <dimension ref="B4:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.125" customWidth="1"/>
-    <col min="2" max="4" width="3.25" customWidth="1"/>
-    <col min="5" max="5" width="22.75" customWidth="1"/>
-    <col min="6" max="6" width="26.625" customWidth="1"/>
+    <col min="2" max="4" width="3.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.75" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
+      <c r="F5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B7" t="s">
+    <row r="7" spans="2:6" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F7" t="s">
-        <v>14</v>
+      <c r="F7" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="C9" t="s">
+    <row r="9" spans="2:6" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F9" t="s">
-        <v>16</v>
+      <c r="F9" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D11" t="s">
+    <row r="11" spans="2:6" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="D11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F11" t="s">
-        <v>17</v>
+      <c r="F11" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="E13" t="s">
+    <row r="13" spans="2:6" ht="81" x14ac:dyDescent="0.15">
+      <c r="E13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F13" t="s">
-        <v>18</v>
+      <c r="F13" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="E15" t="s">
+    <row r="15" spans="2:6" ht="108" x14ac:dyDescent="0.15">
+      <c r="E15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F15" t="s">
-        <v>19</v>
+      <c r="F15" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F16" t="s">
-        <v>20</v>
+      <c r="F16" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D18" t="s">
+    <row r="18" spans="2:6" ht="108" x14ac:dyDescent="0.15">
+      <c r="D18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F18" t="s">
-        <v>21</v>
+      <c r="F18" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="E20" t="s">
+    <row r="20" spans="2:6" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="E20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F20" t="s">
-        <v>22</v>
+      <c r="F20" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F21" t="s">
-        <v>20</v>
+      <c r="F21" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="F24" t="s">
-        <v>23</v>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="E27" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>